<commit_message>
Update occup_isco(*) as string
</commit_message>
<xml_diff>
--- a/Support/Guides and Documentation/GLD_Dictionary_v01.xlsx
+++ b/Support/Guides and Documentation/GLD_Dictionary_v01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb529026\Documents\gld\Support\Guides and Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A805A973-92B9-4464-ABA9-6520A7E31CBB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95035432-0F7E-486E-A8F1-445E1F2DE530}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C416022C-A35E-4942-8219-7CEF6CA35A15}"/>
   </bookViews>
@@ -1744,17 +1744,6 @@
     <t>See industrycat_isic</t>
   </si>
   <si>
-    <t>Four digit integer code</t>
-  </si>
-  <si>
-    <t>ISCO-08 codes are
-8 Plant and machine operators, and assemblers
-   81 Stationary plant machine operators
-      811 Mining and mineral processing plant operators
-         8111 Miners and quarriers
-Given the level of detail available, this are to be coded as 8000, 8100, 8110, and 8111 respectively.</t>
-  </si>
-  <si>
     <t>See occup_isco</t>
   </si>
   <si>
@@ -2068,6 +2057,38 @@
   </si>
   <si>
     <t>Code if there is a single original education variable (as is in most cases). If there are two or more variables, leave missing, make a note of it.</t>
+  </si>
+  <si>
+    <t>ISCO-08 codes are
+8 Plant and machine operators, and assemblers
+   81 Stationary plant machine operators
+      811 Mining and mineral processing plant operators
+         8111 Miners and quarriers
+Given the level of detail available, this are to be coded as 8000, 8100, 8110, and 8111 respectively.
+Note army occupations are coded 0###.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of length four</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -5244,8 +5265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8655A41D-FAAE-4875-A0C4-A516EEA673B9}">
   <dimension ref="A1:F168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5333,29 +5354,29 @@
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="72"/>
       <c r="B5" s="18" t="s">
+        <v>466</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>467</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>468</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>469</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>470</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="20" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="72"/>
       <c r="B6" s="18" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" s="20"/>
@@ -5363,13 +5384,13 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="72"/>
       <c r="B7" s="18" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="20"/>
@@ -5377,13 +5398,13 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="72"/>
       <c r="B8" s="18" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="20"/>
@@ -5858,13 +5879,13 @@
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="78" t="s">
+        <v>484</v>
+      </c>
+      <c r="B39" s="34" t="s">
         <v>486</v>
       </c>
-      <c r="B39" s="34" t="s">
-        <v>488</v>
-      </c>
       <c r="C39" s="35" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D39" s="35" t="s">
         <v>114</v>
@@ -5875,26 +5896,26 @@
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="78"/>
       <c r="B40" s="48" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C40" s="49" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D40" s="49" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E40" s="40"/>
       <c r="F40" s="41" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="78"/>
       <c r="B41" s="38" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C41" s="39" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D41" s="39" t="s">
         <v>108</v>
@@ -5905,45 +5926,45 @@
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="78"/>
       <c r="B42" s="38" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C42" s="39" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D42" s="39" t="s">
         <v>114</v>
       </c>
       <c r="E42" s="40"/>
       <c r="F42" s="41" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="78"/>
       <c r="B43" s="38" t="s">
+        <v>532</v>
+      </c>
+      <c r="C43" s="39" t="s">
         <v>534</v>
       </c>
-      <c r="C43" s="39" t="s">
-        <v>536</v>
-      </c>
       <c r="D43" s="39" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E43" s="40"/>
       <c r="F43" s="41" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="78"/>
       <c r="B44" s="38" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C44" s="38" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D44" s="39" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E44" s="40"/>
       <c r="F44" s="41"/>
@@ -5951,13 +5972,13 @@
     <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="78"/>
       <c r="B45" s="38" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C45" s="38" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D45" s="39" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E45" s="40"/>
       <c r="F45" s="41"/>
@@ -5965,13 +5986,13 @@
     <row r="46" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="78"/>
       <c r="B46" s="46" t="s">
+        <v>492</v>
+      </c>
+      <c r="C46" s="46" t="s">
+        <v>493</v>
+      </c>
+      <c r="D46" s="47" t="s">
         <v>494</v>
-      </c>
-      <c r="C46" s="46" t="s">
-        <v>495</v>
-      </c>
-      <c r="D46" s="47" t="s">
-        <v>496</v>
       </c>
       <c r="E46" s="50"/>
       <c r="F46" s="51"/>
@@ -5979,13 +6000,13 @@
     <row r="47" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="78"/>
       <c r="B47" s="42" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C47" s="42" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D47" s="43" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E47" s="44"/>
       <c r="F47" s="45"/>
@@ -5995,16 +6016,16 @@
         <v>105</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D48" s="24" t="s">
         <v>114</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="F48" s="26"/>
     </row>
@@ -6099,27 +6120,27 @@
         <v>124</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E54" s="32" t="s">
         <v>126</v>
       </c>
       <c r="F54" s="31" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="72"/>
       <c r="B55" s="15" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D55" s="17"/>
       <c r="E55" s="33"/>
       <c r="F55" s="17" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -6128,25 +6149,25 @@
         <v>460</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D56" s="17" t="s">
         <v>461</v>
       </c>
       <c r="E56" s="33"/>
       <c r="F56" s="17" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="73" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B57" s="53" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C57" s="53" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D57" s="54" t="s">
         <v>108</v>
@@ -6157,13 +6178,13 @@
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="73"/>
       <c r="B58" s="53" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C58" s="53" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D58" s="54" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E58" s="55"/>
       <c r="F58" s="54"/>
@@ -6171,10 +6192,10 @@
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="73"/>
       <c r="B59" s="53" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C59" s="53" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D59" s="54" t="s">
         <v>114</v>
@@ -6185,10 +6206,10 @@
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="73"/>
       <c r="B60" s="53" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C60" s="53" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D60" s="54" t="s">
         <v>114</v>
@@ -6199,10 +6220,10 @@
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="73"/>
       <c r="B61" s="53" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C61" s="53" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D61" s="54"/>
       <c r="E61" s="55"/>
@@ -6211,17 +6232,17 @@
     <row r="62" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="73"/>
       <c r="B62" s="53" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C62" s="53" t="s">
+        <v>529</v>
+      </c>
+      <c r="D62" s="54" t="s">
         <v>531</v>
-      </c>
-      <c r="D62" s="54" t="s">
-        <v>533</v>
       </c>
       <c r="E62" s="55"/>
       <c r="F62" s="54" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -6263,33 +6284,33 @@
     <row r="65" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="72"/>
       <c r="B65" s="59" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C65" s="60" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D65" s="60" t="s">
         <v>108</v>
       </c>
       <c r="E65" s="61"/>
       <c r="F65" s="60" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="72"/>
       <c r="B66" s="59" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C66" s="60" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D66" s="60" t="s">
         <v>108</v>
       </c>
       <c r="E66" s="61"/>
       <c r="F66" s="60" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6399,7 +6420,7 @@
         <v>445</v>
       </c>
       <c r="D73" s="59" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E73" s="61"/>
       <c r="F73" s="60" t="s">
@@ -6454,7 +6475,7 @@
       </c>
       <c r="F76" s="60"/>
     </row>
-    <row r="77" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A77" s="72"/>
       <c r="B77" s="59" t="s">
         <v>442</v>
@@ -6463,27 +6484,27 @@
         <v>444</v>
       </c>
       <c r="D77" s="59" t="s">
-        <v>464</v>
+        <v>554</v>
       </c>
       <c r="E77" s="61"/>
       <c r="F77" s="60" t="s">
-        <v>465</v>
+        <v>553</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="72"/>
       <c r="B78" s="59" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C78" s="60" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D78" s="60" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E78" s="61"/>
       <c r="F78" s="60" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="180" x14ac:dyDescent="0.25">
@@ -6793,27 +6814,27 @@
         <v>452</v>
       </c>
       <c r="D98" s="59" t="s">
-        <v>446</v>
+        <v>554</v>
       </c>
       <c r="E98" s="61"/>
       <c r="F98" s="60" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="72"/>
       <c r="B99" s="59" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C99" s="60" t="s">
+        <v>496</v>
+      </c>
+      <c r="D99" s="60" t="s">
         <v>498</v>
-      </c>
-      <c r="D99" s="60" t="s">
-        <v>500</v>
       </c>
       <c r="E99" s="61"/>
       <c r="F99" s="60" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="180" x14ac:dyDescent="0.25">
@@ -6972,7 +6993,7 @@
         <v>459</v>
       </c>
       <c r="C110" s="59" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D110" s="59" t="s">
         <v>39</v>
@@ -6983,7 +7004,7 @@
     <row r="111" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="72"/>
       <c r="B111" s="59" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C111" s="60" t="s">
         <v>422</v>
@@ -7043,33 +7064,33 @@
     <row r="115" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A115" s="72"/>
       <c r="B115" s="59" t="s">
+        <v>510</v>
+      </c>
+      <c r="C115" s="60" t="s">
         <v>512</v>
-      </c>
-      <c r="C115" s="60" t="s">
-        <v>514</v>
       </c>
       <c r="D115" s="60" t="s">
         <v>108</v>
       </c>
       <c r="E115" s="61"/>
       <c r="F115" s="60" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A116" s="72"/>
       <c r="B116" s="59" t="s">
+        <v>511</v>
+      </c>
+      <c r="C116" s="60" t="s">
         <v>513</v>
-      </c>
-      <c r="C116" s="60" t="s">
-        <v>515</v>
       </c>
       <c r="D116" s="60" t="s">
         <v>108</v>
       </c>
       <c r="E116" s="61"/>
       <c r="F116" s="60" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7225,27 +7246,27 @@
         <v>454</v>
       </c>
       <c r="D127" s="59" t="s">
-        <v>446</v>
+        <v>554</v>
       </c>
       <c r="E127" s="61"/>
       <c r="F127" s="60" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="72"/>
       <c r="B128" s="59" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C128" s="60" t="s">
+        <v>496</v>
+      </c>
+      <c r="D128" s="60" t="s">
         <v>498</v>
-      </c>
-      <c r="D128" s="60" t="s">
-        <v>500</v>
       </c>
       <c r="E128" s="61"/>
       <c r="F128" s="60" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="180" x14ac:dyDescent="0.25">
@@ -7449,7 +7470,7 @@
     <row r="143" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A143" s="72"/>
       <c r="B143" s="59" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C143" s="60" t="s">
         <v>402</v>
@@ -7527,27 +7548,27 @@
         <v>458</v>
       </c>
       <c r="D148" s="59" t="s">
-        <v>446</v>
+        <v>554</v>
       </c>
       <c r="E148" s="61"/>
       <c r="F148" s="60" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="149" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A149" s="72"/>
       <c r="B149" s="59" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C149" s="60" t="s">
+        <v>496</v>
+      </c>
+      <c r="D149" s="60" t="s">
         <v>498</v>
-      </c>
-      <c r="D149" s="60" t="s">
-        <v>500</v>
       </c>
       <c r="E149" s="61"/>
       <c r="F149" s="60" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="150" spans="1:6" ht="180" x14ac:dyDescent="0.25">
@@ -7839,48 +7860,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <o1cb080a3dca4eb8a0fd03c7cc8bf8f7 xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </o1cb080a3dca4eb8a0fd03c7cc8bf8f7>
-    <Abstract xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-    <WBDocs_Access_To_Info_Exception xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">12. Not Assessed</WBDocs_Access_To_Info_Exception>
-    <WBDocs_Document_Date xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">2020-12-22T17:31:22+00:00</WBDocs_Document_Date>
-    <TaxCatchAll xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Value>5</Value>
-      <Value>3</Value>
-    </TaxCatchAll>
-    <OneCMS_Subcategory xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-    <i008215bacac45029ee8cafff4c8e93b xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">HSJDR</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b82b4e50-8b87-486b-adae-4a5ffb2d1593</TermId>
-        </TermInfo>
-      </Terms>
-    </i008215bacac45029ee8cafff4c8e93b>
-    <WBDocs_Information_Classification xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">Official Use Only</WBDocs_Information_Classification>
-    <OneCMS_Category xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="WBDocument" ma:contentTypeID="0x010100F4C63C3BD852AE468EAEFD0E6C57C64F020023FF955149D2434D9634B069E3D44A42" ma:contentTypeVersion="49" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="765f642684fa63bc1b9312c368d0b6a5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e02667f-0271-471b-bd6e-11a2e16def1d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e953fe045711556fedbcbd575ad79d22" ns3:_="">
     <xsd:import namespace="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
@@ -8122,44 +8101,54 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <o1cb080a3dca4eb8a0fd03c7cc8bf8f7 xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </o1cb080a3dca4eb8a0fd03c7cc8bf8f7>
+    <Abstract xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+    <WBDocs_Access_To_Info_Exception xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">12. Not Assessed</WBDocs_Access_To_Info_Exception>
+    <WBDocs_Document_Date xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">2020-12-22T17:31:22+00:00</WBDocs_Document_Date>
+    <TaxCatchAll xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Value>5</Value>
+      <Value>3</Value>
+    </TaxCatchAll>
+    <OneCMS_Subcategory xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+    <i008215bacac45029ee8cafff4c8e93b xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">HSJDR</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b82b4e50-8b87-486b-adae-4a5ffb2d1593</TermId>
+        </TermInfo>
+      </Terms>
+    </i008215bacac45029ee8cafff4c8e93b>
+    <WBDocs_Information_Classification xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">Official Use Only</WBDocs_Information_Classification>
+    <OneCMS_Category xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
+</file>
+
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="2a6c10d7-b926-4fc0-945e-3cbf5049f6bd" ContentTypeId="0x010100F4C63C3BD852AE468EAEFD0E6C57C64F02" PreviousValue="false"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B32DBFF-5393-4654-88B0-C956207D28B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8074832C-F0BA-4806-8675-5DC290219507}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33B6C801-2D56-49AD-B646-66F2DEE67E6F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA715D2A-5893-441B-82FC-527C371B80FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8177,6 +8166,38 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33B6C801-2D56-49AD-B646-66F2DEE67E6F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8074832C-F0BA-4806-8675-5DC290219507}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B32DBFF-5393-4654-88B0-C956207D28B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60C49A35-6CF8-4B2E-BB80-5700FA61EE99}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
fixed vars on versions
</commit_message>
<xml_diff>
--- a/Support/Guides and Documentation/GLD_Dictionary_v01.xlsx
+++ b/Support/Guides and Documentation/GLD_Dictionary_v01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb529026\Documents\gld\Support\Guides and Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/aquinonesnunura_worldbank_org/Documents/Documents/GitHub/gld/Support/Guides and Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95035432-0F7E-486E-A8F1-445E1F2DE530}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C416022C-A35E-4942-8219-7CEF6CA35A15}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="19590" windowHeight="10710" activeTab="1" xr2:uid="{C416022C-A35E-4942-8219-7CEF6CA35A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Info and Example" sheetId="1" r:id="rId1"/>
@@ -5265,8 +5265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8655A41D-FAAE-4875-A0C4-A516EEA673B9}">
   <dimension ref="A1:F168"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7860,6 +7860,53 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="2a6c10d7-b926-4fc0-945e-3cbf5049f6bd" ContentTypeId="0x010100F4C63C3BD852AE468EAEFD0E6C57C64F02" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <o1cb080a3dca4eb8a0fd03c7cc8bf8f7 xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </o1cb080a3dca4eb8a0fd03c7cc8bf8f7>
+    <Abstract xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+    <WBDocs_Access_To_Info_Exception xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">12. Not Assessed</WBDocs_Access_To_Info_Exception>
+    <WBDocs_Document_Date xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">2020-12-22T17:31:22+00:00</WBDocs_Document_Date>
+    <TaxCatchAll xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Value>5</Value>
+      <Value>3</Value>
+    </TaxCatchAll>
+    <OneCMS_Subcategory xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+    <i008215bacac45029ee8cafff4c8e93b xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">HSJDR</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b82b4e50-8b87-486b-adae-4a5ffb2d1593</TermId>
+        </TermInfo>
+      </Terms>
+    </i008215bacac45029ee8cafff4c8e93b>
+    <WBDocs_Information_Classification xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">Official Use Only</WBDocs_Information_Classification>
+    <OneCMS_Category xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="WBDocument" ma:contentTypeID="0x010100F4C63C3BD852AE468EAEFD0E6C57C64F020023FF955149D2434D9634B069E3D44A42" ma:contentTypeVersion="49" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="765f642684fa63bc1b9312c368d0b6a5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e02667f-0271-471b-bd6e-11a2e16def1d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e953fe045711556fedbcbd575ad79d22" ns3:_="">
     <xsd:import namespace="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
@@ -8101,54 +8148,47 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <o1cb080a3dca4eb8a0fd03c7cc8bf8f7 xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </o1cb080a3dca4eb8a0fd03c7cc8bf8f7>
-    <Abstract xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-    <WBDocs_Access_To_Info_Exception xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">12. Not Assessed</WBDocs_Access_To_Info_Exception>
-    <WBDocs_Document_Date xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">2020-12-22T17:31:22+00:00</WBDocs_Document_Date>
-    <TaxCatchAll xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Value>5</Value>
-      <Value>3</Value>
-    </TaxCatchAll>
-    <OneCMS_Subcategory xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-    <i008215bacac45029ee8cafff4c8e93b xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">HSJDR</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b82b4e50-8b87-486b-adae-4a5ffb2d1593</TermId>
-        </TermInfo>
-      </Terms>
-    </i008215bacac45029ee8cafff4c8e93b>
-    <WBDocs_Information_Classification xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">Official Use Only</WBDocs_Information_Classification>
-    <OneCMS_Category xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60C49A35-6CF8-4B2E-BB80-5700FA61EE99}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B32DBFF-5393-4654-88B0-C956207D28B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8074832C-F0BA-4806-8675-5DC290219507}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="2a6c10d7-b926-4fc0-945e-3cbf5049f6bd" ContentTypeId="0x010100F4C63C3BD852AE468EAEFD0E6C57C64F02" PreviousValue="false"/>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33B6C801-2D56-49AD-B646-66F2DEE67E6F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA715D2A-5893-441B-82FC-527C371B80FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8164,44 +8204,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33B6C801-2D56-49AD-B646-66F2DEE67E6F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8074832C-F0BA-4806-8675-5DC290219507}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B32DBFF-5393-4654-88B0-C956207D28B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60C49A35-6CF8-4B2E-BB80-5700FA61EE99}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Detail vocational training is in months
</commit_message>
<xml_diff>
--- a/Support/Guides and Documentation/GLD_Dictionary_v01.xlsx
+++ b/Support/Guides and Documentation/GLD_Dictionary_v01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb529026\Documents\gld\Support\Guides and Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C90198-535E-43AC-AD6E-C21818A7245E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF73109C-F8EF-42D1-A7A8-EDDCDD5B9241}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C416022C-A35E-4942-8219-7CEF6CA35A15}"/>
   </bookViews>
@@ -1940,12 +1940,6 @@
     <t>1 = Inside Enterprise; 2 = External</t>
   </si>
   <si>
-    <t>Length of training, lower limit</t>
-  </si>
-  <si>
-    <t>Length of training, upper limit</t>
-  </si>
-  <si>
     <t>Field of training</t>
   </si>
   <si>
@@ -2084,6 +2078,12 @@
   </si>
   <si>
     <t>1 "Low skill" 2 "Medium skill" 3 "High skill"</t>
+  </si>
+  <si>
+    <t>Length of training in months, lower limit</t>
+  </si>
+  <si>
+    <t>Length of training in months, upper limit</t>
   </si>
 </sst>
 </file>
@@ -5260,8 +5260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8655A41D-FAAE-4875-A0C4-A516EEA673B9}">
   <dimension ref="A1:F168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="D156" sqref="D156"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5365,13 +5365,13 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="72"/>
       <c r="B6" s="18" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" s="20"/>
@@ -5379,13 +5379,13 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="72"/>
       <c r="B7" s="18" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="20"/>
@@ -5393,13 +5393,13 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="72"/>
       <c r="B8" s="18" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="20"/>
@@ -5937,13 +5937,13 @@
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="78"/>
       <c r="B43" s="38" t="s">
+        <v>529</v>
+      </c>
+      <c r="C43" s="39" t="s">
         <v>531</v>
       </c>
-      <c r="C43" s="39" t="s">
-        <v>533</v>
-      </c>
       <c r="D43" s="39" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E43" s="40"/>
       <c r="F43" s="41" t="s">
@@ -5959,7 +5959,7 @@
         <v>479</v>
       </c>
       <c r="D44" s="39" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E44" s="40"/>
       <c r="F44" s="41"/>
@@ -6115,27 +6115,27 @@
         <v>124</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E54" s="32" t="s">
         <v>126</v>
       </c>
       <c r="F54" s="31" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="72"/>
       <c r="B55" s="15" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D55" s="17"/>
       <c r="E55" s="33"/>
       <c r="F55" s="17" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -6151,7 +6151,7 @@
       </c>
       <c r="E56" s="33"/>
       <c r="F56" s="17" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -6190,7 +6190,7 @@
         <v>517</v>
       </c>
       <c r="C59" s="53" t="s">
-        <v>525</v>
+        <v>552</v>
       </c>
       <c r="D59" s="54" t="s">
         <v>114</v>
@@ -6204,7 +6204,7 @@
         <v>518</v>
       </c>
       <c r="C60" s="53" t="s">
-        <v>526</v>
+        <v>553</v>
       </c>
       <c r="D60" s="54" t="s">
         <v>114</v>
@@ -6218,7 +6218,7 @@
         <v>519</v>
       </c>
       <c r="C61" s="53" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D61" s="54"/>
       <c r="E61" s="55"/>
@@ -6230,14 +6230,14 @@
         <v>520</v>
       </c>
       <c r="C62" s="53" t="s">
+        <v>526</v>
+      </c>
+      <c r="D62" s="54" t="s">
         <v>528</v>
-      </c>
-      <c r="D62" s="54" t="s">
-        <v>530</v>
       </c>
       <c r="E62" s="55"/>
       <c r="F62" s="54" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -6415,7 +6415,7 @@
         <v>445</v>
       </c>
       <c r="D73" s="59" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="E73" s="61"/>
       <c r="F73" s="60" t="s">
@@ -6479,11 +6479,11 @@
         <v>444</v>
       </c>
       <c r="D77" s="59" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E77" s="61"/>
       <c r="F77" s="60" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6495,7 +6495,7 @@
         <v>496</v>
       </c>
       <c r="D78" s="60" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="E78" s="61"/>
       <c r="F78" s="60" t="s">
@@ -6809,7 +6809,7 @@
         <v>452</v>
       </c>
       <c r="D98" s="59" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E98" s="61"/>
       <c r="F98" s="60" t="s">
@@ -6825,7 +6825,7 @@
         <v>496</v>
       </c>
       <c r="D99" s="60" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="E99" s="61"/>
       <c r="F99" s="60" t="s">
@@ -7241,7 +7241,7 @@
         <v>454</v>
       </c>
       <c r="D127" s="59" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E127" s="61"/>
       <c r="F127" s="60" t="s">
@@ -7257,7 +7257,7 @@
         <v>496</v>
       </c>
       <c r="D128" s="60" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="E128" s="61"/>
       <c r="F128" s="60" t="s">
@@ -7543,7 +7543,7 @@
         <v>458</v>
       </c>
       <c r="D148" s="59" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E148" s="61"/>
       <c r="F148" s="60" t="s">
@@ -7559,7 +7559,7 @@
         <v>496</v>
       </c>
       <c r="D149" s="60" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="E149" s="61"/>
       <c r="F149" s="60" t="s">
@@ -7855,6 +7855,53 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="2a6c10d7-b926-4fc0-945e-3cbf5049f6bd" ContentTypeId="0x010100F4C63C3BD852AE468EAEFD0E6C57C64F02" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <o1cb080a3dca4eb8a0fd03c7cc8bf8f7 xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </o1cb080a3dca4eb8a0fd03c7cc8bf8f7>
+    <Abstract xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+    <WBDocs_Access_To_Info_Exception xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">12. Not Assessed</WBDocs_Access_To_Info_Exception>
+    <WBDocs_Document_Date xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">2020-12-22T17:31:22+00:00</WBDocs_Document_Date>
+    <TaxCatchAll xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Value>5</Value>
+      <Value>3</Value>
+    </TaxCatchAll>
+    <OneCMS_Subcategory xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+    <i008215bacac45029ee8cafff4c8e93b xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">HSJDR</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b82b4e50-8b87-486b-adae-4a5ffb2d1593</TermId>
+        </TermInfo>
+      </Terms>
+    </i008215bacac45029ee8cafff4c8e93b>
+    <WBDocs_Information_Classification xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">Official Use Only</WBDocs_Information_Classification>
+    <OneCMS_Category xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="WBDocument" ma:contentTypeID="0x010100F4C63C3BD852AE468EAEFD0E6C57C64F020023FF955149D2434D9634B069E3D44A42" ma:contentTypeVersion="49" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="765f642684fa63bc1b9312c368d0b6a5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e02667f-0271-471b-bd6e-11a2e16def1d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e953fe045711556fedbcbd575ad79d22" ns3:_="">
     <xsd:import namespace="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
@@ -8096,54 +8143,47 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <o1cb080a3dca4eb8a0fd03c7cc8bf8f7 xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </o1cb080a3dca4eb8a0fd03c7cc8bf8f7>
-    <Abstract xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-    <WBDocs_Access_To_Info_Exception xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">12. Not Assessed</WBDocs_Access_To_Info_Exception>
-    <WBDocs_Document_Date xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">2020-12-22T17:31:22+00:00</WBDocs_Document_Date>
-    <TaxCatchAll xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Value>5</Value>
-      <Value>3</Value>
-    </TaxCatchAll>
-    <OneCMS_Subcategory xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-    <i008215bacac45029ee8cafff4c8e93b xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">HSJDR</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b82b4e50-8b87-486b-adae-4a5ffb2d1593</TermId>
-        </TermInfo>
-      </Terms>
-    </i008215bacac45029ee8cafff4c8e93b>
-    <WBDocs_Information_Classification xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d">Official Use Only</WBDocs_Information_Classification>
-    <OneCMS_Category xmlns="3e02667f-0271-471b-bd6e-11a2e16def1d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60C49A35-6CF8-4B2E-BB80-5700FA61EE99}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B32DBFF-5393-4654-88B0-C956207D28B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8074832C-F0BA-4806-8675-5DC290219507}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="2a6c10d7-b926-4fc0-945e-3cbf5049f6bd" ContentTypeId="0x010100F4C63C3BD852AE468EAEFD0E6C57C64F02" PreviousValue="false"/>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33B6C801-2D56-49AD-B646-66F2DEE67E6F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA715D2A-5893-441B-82FC-527C371B80FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8159,44 +8199,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33B6C801-2D56-49AD-B646-66F2DEE67E6F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3e02667f-0271-471b-bd6e-11a2e16def1d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8074832C-F0BA-4806-8675-5DC290219507}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B32DBFF-5393-4654-88B0-C956207D28B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60C49A35-6CF8-4B2E-BB80-5700FA61EE99}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>